<commit_message>
Updated template and code.
</commit_message>
<xml_diff>
--- a/data/table_data.xlsx
+++ b/data/table_data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pwcapac-my.sharepoint.com/personal/prasanthi_r_ramaswamy_pwc_com/Documents/Proposals and RFPs/SIT/Grant Research Assistant Files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="49" documentId="11_21FA65B191E6E8BF891C87DDD26A5DA3C0385FCA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66E79516-5B6C-4950-87D1-114EA2F1D083}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28695" yWindow="1920" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
   <si>
     <t>Proposal Section</t>
   </si>
@@ -22,36 +28,9 @@
     <t>Included</t>
   </si>
   <si>
-    <t>Cover Letter</t>
-  </si>
-  <si>
-    <t>Introduction</t>
-  </si>
-  <si>
-    <t>Scientific Objectives</t>
-  </si>
-  <si>
     <t>Methodology</t>
   </si>
   <si>
-    <t>Expected Outcomes</t>
-  </si>
-  <si>
-    <t>Relevance to Funding Priorities</t>
-  </si>
-  <si>
-    <t>Personnel &amp; Team Composition</t>
-  </si>
-  <si>
-    <t>Workplan &amp; Milestones</t>
-  </si>
-  <si>
-    <t>Ethics &amp; Regulatory Considerations</t>
-  </si>
-  <si>
-    <t>Detailed Budget</t>
-  </si>
-  <si>
     <t>Appendices</t>
   </si>
   <si>
@@ -59,13 +38,61 @@
   </si>
   <si>
     <t>✅</t>
+  </si>
+  <si>
+    <t>General Information</t>
+  </si>
+  <si>
+    <t>Scientific Abstract of the Proposal</t>
+  </si>
+  <si>
+    <t>Objectives</t>
+  </si>
+  <si>
+    <t>Expected Scientific Results of the Joint Research</t>
+  </si>
+  <si>
+    <t>Expected Economic and Social Impact of the Joint Research</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>Research Topic and Work Plan</t>
+  </si>
+  <si>
+    <t>Detailed Description of Joint Project</t>
+  </si>
+  <si>
+    <t>Future Prospect of Research</t>
+  </si>
+  <si>
+    <t>Bibliography</t>
+  </si>
+  <si>
+    <t>Work Contribution</t>
+  </si>
+  <si>
+    <t>Problem Statement</t>
+  </si>
+  <si>
+    <t>Budget Description</t>
+  </si>
+  <si>
+    <t>Curriculum Vitae</t>
+  </si>
+  <si>
+    <t>Acknowledgment</t>
+  </si>
+  <si>
+    <t>Section</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,10 +144,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -128,13 +158,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -172,7 +210,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -206,6 +244,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -240,9 +279,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -415,107 +455,211 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="54.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>